<commit_message>
MedDRA vis POC with /r/vis/MedraCollapsible.R
</commit_message>
<xml_diff>
--- a/r/MedDRA_Subsetting_To_OntInstanceData.xlsx
+++ b/r/MedDRA_Subsetting_To_OntInstanceData.xlsx
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,13 +109,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -139,6 +152,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,19 +470,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -473,12 +490,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -496,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -513,7 +530,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>10003058</v>
+      </c>
       <c r="C5" s="4">
         <v>10003041</v>
       </c>
@@ -527,7 +547,7 @@
         <v>10018065</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C6" s="4"/>
       <c r="E6" s="4">
         <v>10001316</v>
@@ -536,7 +556,7 @@
         <v>10022117</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C7" s="4">
         <v>10003041</v>
       </c>
@@ -550,60 +570,58 @@
         <v>10040785</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="7">
         <v>10003047</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>10003053</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>10049293</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8">
         <v>10014982</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <v>10040785</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>10003053</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>10003057</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="9">
         <v>10001316</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="8">
         <v>10018065</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="E11" s="4">
+      <c r="E11" s="9">
         <v>10001316</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="8">
         <v>10022117</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>10003058</v>
-      </c>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
+        <v>10003851</v>
+      </c>
       <c r="C13" s="1">
         <v>10003677</v>
       </c>
@@ -617,20 +635,16 @@
         <v>10007541</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <v>10003851</v>
-      </c>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
         <v>10012727</v>
       </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
       <c r="C16" s="1">
         <v>10012735</v>
       </c>
@@ -644,7 +658,7 @@
         <v>10017947</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C17" s="1">
         <v>10015150</v>
       </c>
@@ -658,9 +672,26 @@
         <v>10040785</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C19" s="6">
         <v>10024781</v>
+      </c>
+      <c r="D19">
+        <v>10015151</v>
+      </c>
+      <c r="E19">
+        <v>10014982</v>
+      </c>
+      <c r="F19">
+        <v>10040785</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>10003041</v>
+      </c>
+      <c r="F20">
+        <v>10003057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>